<commit_message>
Small 2-region data adjusted for taxes
Tax layer is adjusted in order ensure that tax rate is the same for
domestic and imported product
</commit_message>
<xml_diff>
--- a/data/SAMdata_closed_economy_matrix_format.xlsx
+++ b/data/SAMdata_closed_economy_matrix_format.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">tax_layer!$AH$45:$AH$52</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">tax_layer!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
@@ -28,7 +28,7 @@
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">tax_layer!$AH$70</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">tax_layer!$AH$58</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
@@ -194,7 +194,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,10 +474,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -495,7 +503,18 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -542,8 +561,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -842,7 +862,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP72"/>
+  <dimension ref="A1:AQ56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
@@ -858,17 +878,18 @@
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="35" width="9" customWidth="1"/>
     <col min="36" max="36" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="14.85546875" customWidth="1"/>
     <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -876,7 +897,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -884,52 +905,52 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="E4" s="39" t="s">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="E4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="25" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="25" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="25" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="27"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="38"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1024,11 +1045,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1123,14 +1144,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1225,8 +1246,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -1310,34 +1331,34 @@
       <c r="AB8" s="22">
         <v>0</v>
       </c>
-      <c r="AC8" s="10">
-        <v>106724.18362976026</v>
-      </c>
-      <c r="AD8" s="10">
+      <c r="AC8" s="24">
+        <v>104388.20943174293</v>
+      </c>
+      <c r="AD8" s="24">
         <v>1935.0985801925456</v>
       </c>
-      <c r="AE8" s="10">
+      <c r="AE8" s="24">
         <v>16103.213972799878</v>
       </c>
-      <c r="AF8" s="13">
-        <v>1284.4988073369193</v>
-      </c>
-      <c r="AG8" s="13">
+      <c r="AF8" s="27">
+        <v>3620.4730053542426</v>
+      </c>
+      <c r="AG8" s="27">
         <v>23.54478465587021</v>
       </c>
-      <c r="AH8" s="13">
+      <c r="AH8" s="27">
         <v>195.93146785278896</v>
       </c>
-      <c r="AI8" s="13">
+      <c r="AI8" s="27">
         <v>0</v>
       </c>
       <c r="AK8" s="17"/>
-      <c r="AL8" s="17">
-        <v>1153.8055325891473</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="AL8" s="17"/>
+      <c r="AM8" s="31"/>
+      <c r="AN8" s="31"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1419,34 +1440,34 @@
       <c r="AB9" s="18">
         <v>0</v>
       </c>
-      <c r="AC9" s="11">
-        <v>2183927.2015514718</v>
-      </c>
-      <c r="AD9" s="11">
+      <c r="AC9" s="25">
+        <v>2051375.1268372941</v>
+      </c>
+      <c r="AD9" s="25">
         <v>54558.117734633946</v>
       </c>
-      <c r="AE9" s="11">
+      <c r="AE9" s="25">
         <v>632906.35752765276</v>
       </c>
-      <c r="AF9" s="12">
-        <v>72887.355530256944</v>
-      </c>
-      <c r="AG9" s="12">
+      <c r="AF9" s="26">
+        <v>205439.43024443468</v>
+      </c>
+      <c r="AG9" s="26">
         <v>2800.4487586910768</v>
       </c>
-      <c r="AH9" s="12">
+      <c r="AH9" s="26">
         <v>32486.857994751856</v>
       </c>
-      <c r="AI9" s="12">
+      <c r="AI9" s="26">
         <v>0</v>
       </c>
       <c r="AK9" s="17"/>
-      <c r="AL9">
-        <v>763941.59672843106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="AL9" s="31"/>
+      <c r="AM9" s="31"/>
+      <c r="AN9" s="31"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1528,34 +1549,34 @@
       <c r="AB10" s="18">
         <v>0</v>
       </c>
-      <c r="AC10" s="11">
-        <v>49594.661048285867</v>
-      </c>
-      <c r="AD10" s="11">
+      <c r="AC10" s="25">
+        <v>49573.496389031883</v>
+      </c>
+      <c r="AD10" s="25">
         <v>4102.8475336669308</v>
       </c>
-      <c r="AE10" s="11">
+      <c r="AE10" s="25">
         <v>1182390.8948782317</v>
       </c>
-      <c r="AF10" s="12">
-        <v>11.637962265383223</v>
-      </c>
-      <c r="AG10" s="12">
+      <c r="AF10" s="26">
+        <v>32.802621519366994</v>
+      </c>
+      <c r="AG10" s="26">
         <v>1.011996718728976</v>
       </c>
-      <c r="AH10" s="12">
+      <c r="AH10" s="26">
         <v>291.64517961074347</v>
       </c>
-      <c r="AI10" s="12">
+      <c r="AI10" s="26">
         <v>0</v>
       </c>
       <c r="AK10" s="17"/>
-      <c r="AL10" s="17">
-        <v>2411.9144111161586</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="AL10" s="31"/>
+      <c r="AM10" s="31"/>
+      <c r="AN10" s="31"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1637,34 +1658,34 @@
       <c r="AB11" s="18">
         <v>0</v>
       </c>
-      <c r="AC11" s="11">
-        <v>4632010.7397648115</v>
-      </c>
-      <c r="AD11" s="11">
+      <c r="AC11" s="25">
+        <v>4574761.4834305905</v>
+      </c>
+      <c r="AD11" s="25">
         <v>2473551.1538742785</v>
       </c>
-      <c r="AE11" s="11">
+      <c r="AE11" s="25">
         <v>494454.62593600858</v>
       </c>
-      <c r="AF11" s="12">
-        <v>31480.0572474851</v>
-      </c>
-      <c r="AG11" s="12">
+      <c r="AF11" s="26">
+        <v>88729.313581706883</v>
+      </c>
+      <c r="AG11" s="26">
         <v>17707.532201710368</v>
       </c>
-      <c r="AH11" s="12">
+      <c r="AH11" s="26">
         <v>3539.6766294211593</v>
       </c>
-      <c r="AI11" s="12">
+      <c r="AI11" s="26">
         <v>0</v>
       </c>
       <c r="AK11" s="17"/>
-      <c r="AL11">
-        <v>234586.46621053852</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="AL11" s="31"/>
+      <c r="AM11" s="31"/>
+      <c r="AN11" s="31"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1746,34 +1767,34 @@
       <c r="AB12" s="18">
         <v>0</v>
       </c>
-      <c r="AC12" s="12">
-        <v>6183.7548498922661</v>
-      </c>
-      <c r="AD12" s="12">
-        <v>113.34784857236332</v>
-      </c>
-      <c r="AE12" s="12">
-        <v>819.49375627442464</v>
-      </c>
-      <c r="AF12" s="11">
+      <c r="AC12" s="26">
+        <v>6068.0377839299081</v>
+      </c>
+      <c r="AD12" s="26">
+        <v>112.4863752732101</v>
+      </c>
+      <c r="AE12" s="26">
+        <v>936.07229553593652</v>
+      </c>
+      <c r="AF12" s="25">
         <v>47954.201734266717</v>
       </c>
-      <c r="AG12" s="11">
+      <c r="AG12" s="25">
         <v>729.04796471360805</v>
       </c>
-      <c r="AH12" s="11">
+      <c r="AH12" s="25">
         <v>-33.564392557460792</v>
       </c>
-      <c r="AI12" s="12">
+      <c r="AI12" s="26">
         <v>0</v>
       </c>
       <c r="AK12" s="17"/>
-      <c r="AL12">
-        <v>8180.5849926687661</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="AL12" s="31"/>
+      <c r="AM12" s="31"/>
+      <c r="AN12" s="31"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1855,34 +1876,34 @@
       <c r="AB13" s="18">
         <v>0</v>
       </c>
-      <c r="AC13" s="12">
-        <v>124268.16654204736</v>
-      </c>
-      <c r="AD13" s="12">
-        <v>4774.5816843777284</v>
-      </c>
-      <c r="AE13" s="12">
-        <v>80809.185823161592</v>
-      </c>
-      <c r="AF13" s="11">
+      <c r="AC13" s="26">
+        <v>157177.89296533272</v>
+      </c>
+      <c r="AD13" s="26">
+        <v>4180.283692386055</v>
+      </c>
+      <c r="AE13" s="26">
+        <v>48493.757391867912</v>
+      </c>
+      <c r="AF13" s="25">
         <v>1109394.8579546527</v>
       </c>
-      <c r="AG13" s="11">
+      <c r="AG13" s="25">
         <v>39807.951174906972</v>
       </c>
-      <c r="AH13" s="11">
+      <c r="AH13" s="25">
         <v>375081.30807734397</v>
       </c>
-      <c r="AI13" s="12">
+      <c r="AI13" s="26">
         <v>0</v>
       </c>
       <c r="AK13" s="17"/>
-      <c r="AL13" s="17">
-        <v>73312.236834776588</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="AL13" s="31"/>
+      <c r="AM13" s="31"/>
+      <c r="AN13" s="31"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1964,34 +1985,34 @@
       <c r="AB14" s="18">
         <v>0</v>
       </c>
-      <c r="AC14" s="12">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="12">
-        <v>0</v>
-      </c>
-      <c r="AE14" s="12">
-        <v>10</v>
-      </c>
-      <c r="AF14" s="11">
+      <c r="AC14" s="26">
+        <v>0.40105825017352253</v>
+      </c>
+      <c r="AD14" s="26">
+        <v>3.3192753637309988E-2</v>
+      </c>
+      <c r="AE14" s="26">
+        <v>9.5657489961891677</v>
+      </c>
+      <c r="AF14" s="25">
         <v>45.404385260888375</v>
       </c>
-      <c r="AG14" s="11">
-        <v>0</v>
-      </c>
-      <c r="AH14" s="11">
+      <c r="AG14" s="25">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="25">
         <v>879077.25282743527</v>
       </c>
-      <c r="AI14" s="12">
+      <c r="AI14" s="26">
         <v>0</v>
       </c>
       <c r="AK14" s="17"/>
-      <c r="AL14">
-        <v>45.404385260888375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="AL14" s="31"/>
+      <c r="AM14" s="31"/>
+      <c r="AN14" s="31"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -2073,35 +2094,35 @@
       <c r="AB15" s="18">
         <v>0</v>
       </c>
-      <c r="AC15" s="12">
-        <v>11554.155963616675</v>
-      </c>
-      <c r="AD15" s="12">
-        <v>6499.2127295343789</v>
-      </c>
-      <c r="AE15" s="12">
-        <v>4220.0397558438808</v>
-      </c>
-      <c r="AF15" s="11">
+      <c r="AC15" s="26">
+        <v>13509.038197925038</v>
+      </c>
+      <c r="AD15" s="26">
+        <v>7304.2708659755572</v>
+      </c>
+      <c r="AE15" s="26">
+        <v>1460.0993850943401</v>
+      </c>
+      <c r="AF15" s="25">
         <v>5844935.1802719012</v>
       </c>
-      <c r="AG15" s="11">
+      <c r="AG15" s="25">
         <v>1533703.7650708512</v>
       </c>
-      <c r="AH15" s="11">
+      <c r="AH15" s="25">
         <v>470917.6438234222</v>
       </c>
-      <c r="AI15" s="12">
+      <c r="AI15" s="26">
         <v>0</v>
       </c>
       <c r="AJ15" s="17"/>
       <c r="AK15" s="17"/>
-      <c r="AL15">
-        <v>3118350.7090348322</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="AL15" s="31"/>
+      <c r="AM15" s="31"/>
+      <c r="AN15" s="31"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -2206,12 +2227,12 @@
       <c r="AI16" s="18">
         <v>0</v>
       </c>
-      <c r="AL16">
-        <v>0</v>
-      </c>
+      <c r="AL16" s="31"/>
+      <c r="AM16" s="31"/>
+      <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -2314,12 +2335,12 @@
       <c r="AI17" s="18">
         <v>0</v>
       </c>
-      <c r="AL17">
-        <v>0</v>
-      </c>
+      <c r="AL17" s="31"/>
+      <c r="AM17" s="31"/>
+      <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2422,12 +2443,12 @@
       <c r="AI18" s="18">
         <v>0</v>
       </c>
-      <c r="AL18">
-        <v>0</v>
-      </c>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2530,12 +2551,12 @@
       <c r="AI19" s="18">
         <v>0</v>
       </c>
-      <c r="AL19">
-        <v>0</v>
-      </c>
+      <c r="AL19" s="31"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -2638,12 +2659,12 @@
       <c r="AI20" s="18">
         <v>0</v>
       </c>
-      <c r="AL20">
-        <v>0</v>
-      </c>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -2746,12 +2767,12 @@
       <c r="AI21" s="18">
         <v>0</v>
       </c>
-      <c r="AL21">
-        <v>0</v>
-      </c>
+      <c r="AL21" s="31"/>
+      <c r="AM21" s="31"/>
+      <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -2854,12 +2875,12 @@
       <c r="AI22" s="18">
         <v>0</v>
       </c>
-      <c r="AL22">
-        <v>0</v>
-      </c>
+      <c r="AL22" s="31"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -2962,12 +2983,12 @@
       <c r="AI23" s="18">
         <v>0</v>
       </c>
-      <c r="AL23">
-        <v>0</v>
-      </c>
+      <c r="AL23" s="31"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -3052,13 +3073,13 @@
         <v>0</v>
       </c>
       <c r="AC24" s="9">
-        <v>802703.11982013995</v>
+        <v>800641.44389313203</v>
       </c>
       <c r="AD24" s="9">
         <v>0</v>
       </c>
       <c r="AE24" s="9">
-        <v>204412.67687368783</v>
+        <v>199824.36184873641</v>
       </c>
       <c r="AF24" s="9">
         <v>0</v>
@@ -3072,12 +3093,12 @@
       <c r="AI24" s="9">
         <v>0</v>
       </c>
-      <c r="AL24">
-        <v>0</v>
-      </c>
+      <c r="AL24" s="31"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -3180,12 +3201,12 @@
       <c r="AI25" s="9">
         <v>0</v>
       </c>
-      <c r="AL25">
-        <v>0</v>
-      </c>
+      <c r="AL25" s="31"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -3288,12 +3309,12 @@
       <c r="AI26" s="9">
         <v>0</v>
       </c>
-      <c r="AL26">
-        <v>0</v>
-      </c>
+      <c r="AL26" s="31"/>
+      <c r="AM26" s="31"/>
+      <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -3396,12 +3417,12 @@
       <c r="AI27" s="9">
         <v>0</v>
       </c>
-      <c r="AL27">
-        <v>0</v>
-      </c>
+      <c r="AL27" s="31"/>
+      <c r="AM27" s="31"/>
+      <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -3504,12 +3525,12 @@
       <c r="AI28" s="9">
         <v>0</v>
       </c>
-      <c r="AL28">
-        <v>0</v>
-      </c>
+      <c r="AL28" s="31"/>
+      <c r="AM28" s="31"/>
+      <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -3612,12 +3633,12 @@
       <c r="AI29" s="9">
         <v>0</v>
       </c>
-      <c r="AL29">
-        <v>0</v>
-      </c>
+      <c r="AL29" s="31"/>
+      <c r="AM29" s="31"/>
+      <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -3720,12 +3741,12 @@
       <c r="AI30" s="9">
         <v>0</v>
       </c>
-      <c r="AL30">
-        <v>0</v>
-      </c>
+      <c r="AL30" s="31"/>
+      <c r="AM30" s="31"/>
+      <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -3828,12 +3849,12 @@
       <c r="AI31" s="9">
         <v>0</v>
       </c>
-      <c r="AL31">
-        <v>0</v>
-      </c>
+      <c r="AL31" s="31"/>
+      <c r="AM31" s="31"/>
+      <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -3919,38 +3940,37 @@
       <c r="AB32" s="9">
         <v>0</v>
       </c>
-      <c r="AC32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD32" s="9">
+      <c r="AC32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="30">
         <v>396715.17018065182</v>
       </c>
-      <c r="AE32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF32" s="9">
-        <v>292158.46990567073</v>
-      </c>
-      <c r="AG32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH32" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI32" s="24">
+      <c r="AE32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="30">
+        <v>100000</v>
+      </c>
+      <c r="AG32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="32">
         <v>0</v>
       </c>
       <c r="AJ32" s="17"/>
       <c r="AK32" s="17"/>
-      <c r="AL32">
-        <v>-97696.032680971548</v>
-      </c>
-      <c r="AN32" s="17"/>
+      <c r="AL32" s="31"/>
+      <c r="AM32" s="31"/>
+      <c r="AN32" s="31"/>
       <c r="AO32" s="17"/>
       <c r="AP32" s="17"/>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -4010,7 +4030,7 @@
       </c>
       <c r="U33" s="9">
         <f>SUM(M24:P24)+SUM(AC24:AE24)</f>
-        <v>1376928.2334026387</v>
+        <v>1370278.2424506797</v>
       </c>
       <c r="V33" s="9">
         <v>0</v>
@@ -4034,37 +4054,36 @@
       <c r="AB33" s="9">
         <v>0</v>
       </c>
-      <c r="AC33" s="9">
-        <v>1666879.5468354388</v>
-      </c>
-      <c r="AD33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI33" s="9">
+      <c r="AC33" s="30">
+        <v>1403430.519579133</v>
+      </c>
+      <c r="AD33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH33" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI33" s="30">
         <v>0</v>
       </c>
       <c r="AJ33" s="17"/>
-      <c r="AL33">
-        <v>0</v>
-      </c>
-      <c r="AN33" s="17"/>
+      <c r="AL33" s="31"/>
+      <c r="AM33" s="31"/>
+      <c r="AN33" s="31"/>
       <c r="AO33" s="17"/>
       <c r="AP33" s="17"/>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -4146,37 +4165,36 @@
       <c r="AB34" s="9">
         <v>0</v>
       </c>
-      <c r="AC34" s="9">
-        <v>2345817.5384514933</v>
-      </c>
-      <c r="AD34" s="9">
-        <v>270308.95007216698</v>
-      </c>
-      <c r="AE34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI34" s="9">
+      <c r="AC34" s="30">
+        <v>2576578.9489849228</v>
+      </c>
+      <c r="AD34" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="30">
         <v>0</v>
       </c>
       <c r="AJ34" s="17"/>
-      <c r="AL34">
-        <v>0</v>
-      </c>
-      <c r="AN34" s="17"/>
+      <c r="AL34" s="31"/>
+      <c r="AM34" s="31"/>
+      <c r="AN34" s="31"/>
       <c r="AO34" s="17"/>
       <c r="AP34" s="17"/>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -4260,37 +4278,36 @@
         <f>SUM(Q31:T31)</f>
         <v>4988422.5814544149</v>
       </c>
-      <c r="AC35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG35" s="9">
+      <c r="AC35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG35" s="30">
         <v>316171.98370718816</v>
       </c>
-      <c r="AH35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI35" s="24">
+      <c r="AH35" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI35" s="32">
         <v>0</v>
       </c>
       <c r="AK35" s="17"/>
-      <c r="AL35">
-        <v>1514896.0133418497</v>
-      </c>
-      <c r="AN35" s="17"/>
+      <c r="AL35" s="31"/>
+      <c r="AM35" s="31"/>
+      <c r="AN35" s="31"/>
       <c r="AO35" s="17"/>
       <c r="AP35" s="17"/>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -4374,37 +4391,37 @@
       <c r="AB36" s="9">
         <v>0</v>
       </c>
-      <c r="AC36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF36" s="9">
-        <v>1840871.1526996384</v>
-      </c>
-      <c r="AG36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI36" s="9">
+      <c r="AC36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF36" s="30">
+        <v>1840871.1526996386</v>
+      </c>
+      <c r="AG36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH36" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI36" s="30">
         <v>0</v>
       </c>
       <c r="AJ36" s="17"/>
-      <c r="AL36">
-        <v>0</v>
-      </c>
-      <c r="AN36" s="17"/>
+      <c r="AK36" s="28"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="31"/>
       <c r="AO36" s="17"/>
       <c r="AP36" s="17"/>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -4486,37 +4503,36 @@
       <c r="AB37" s="9">
         <v>0</v>
       </c>
-      <c r="AC37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF37" s="9">
+      <c r="AC37" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF37" s="30">
         <v>1624019.4891072803</v>
       </c>
-      <c r="AG37" s="9">
+      <c r="AG37" s="30">
         <v>137537.26250000019</v>
       </c>
-      <c r="AH37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI37" s="9">
+      <c r="AH37" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI37" s="30">
         <v>0</v>
       </c>
       <c r="AJ37" s="17"/>
-      <c r="AL37">
-        <v>0</v>
-      </c>
-      <c r="AN37" s="17"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
       <c r="AO37" s="17"/>
       <c r="AP37" s="17"/>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="45"/>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
@@ -4598,32 +4614,32 @@
       <c r="AB38" s="9">
         <v>0</v>
       </c>
-      <c r="AC38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AD38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AE38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AF38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AG38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AH38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AI38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AL38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AI38" s="30">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+    </row>
+    <row r="40" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
       <c r="O40" s="17"/>
@@ -4633,90 +4649,97 @@
       <c r="S40" s="17"/>
       <c r="T40" s="17"/>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-      <c r="L41" s="17"/>
-      <c r="M41" s="17">
-        <v>3392.9708317052609</v>
-      </c>
-      <c r="N41" s="17">
-        <v>197334.18448755972</v>
-      </c>
-      <c r="O41" s="17">
-        <v>12743.89411571547</v>
-      </c>
-      <c r="P41" s="17">
-        <v>158355.57893565058</v>
-      </c>
-      <c r="Q41" s="17">
-        <v>5907.1633783290745</v>
-      </c>
-      <c r="R41" s="17">
-        <v>308796.03558555245</v>
-      </c>
-      <c r="S41" s="17">
-        <v>31427.424968989566</v>
-      </c>
-      <c r="T41" s="17">
-        <v>151474.85676760226</v>
-      </c>
-      <c r="AC41">
-        <v>133501.18656283186</v>
-      </c>
-      <c r="AD41">
-        <v>19948.453164561084</v>
-      </c>
-      <c r="AE41">
-        <v>86963.012198008553</v>
-      </c>
-      <c r="AF41">
-        <v>3062530.012279626</v>
-      </c>
-      <c r="AG41">
-        <v>457619.42712224292</v>
-      </c>
-      <c r="AH41">
-        <v>989188.49839271954</v>
-      </c>
-    </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="31"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AC42" s="17"/>
       <c r="AF42" s="17"/>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="AC43" s="17"/>
-      <c r="AD43" s="17"/>
-      <c r="AE43" s="17"/>
-      <c r="AF43" s="17"/>
-      <c r="AG43" s="17"/>
-      <c r="AH43" s="17"/>
-    </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AI43" s="33"/>
+      <c r="AJ43" s="33"/>
+      <c r="AK43" s="33"/>
+      <c r="AM43" s="34"/>
+      <c r="AO43" s="35"/>
+      <c r="AP43" s="35"/>
+      <c r="AQ43" s="35"/>
+    </row>
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17"/>
       <c r="P44" s="17"/>
-    </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-    </row>
-    <row r="60" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M60" s="17"/>
-      <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="17"/>
-    </row>
-    <row r="72" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M72" s="17"/>
+      <c r="AI44" s="33"/>
+      <c r="AJ44" s="33"/>
+      <c r="AK44" s="33"/>
+      <c r="AM44" s="34"/>
+      <c r="AO44" s="35"/>
+      <c r="AP44" s="35"/>
+      <c r="AQ44" s="35"/>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AC45" s="31"/>
+      <c r="AD45" s="31"/>
+      <c r="AE45" s="31"/>
+      <c r="AI45" s="33"/>
+      <c r="AJ45" s="33"/>
+      <c r="AK45" s="33"/>
+      <c r="AM45" s="34"/>
+      <c r="AO45" s="35"/>
+      <c r="AP45" s="35"/>
+      <c r="AQ45" s="35"/>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AI46" s="33"/>
+      <c r="AJ46" s="33"/>
+      <c r="AK46" s="33"/>
+      <c r="AM46" s="34"/>
+      <c r="AO46" s="35"/>
+      <c r="AP46" s="35"/>
+      <c r="AQ46" s="35"/>
+    </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AI47" s="33"/>
+      <c r="AJ47" s="33"/>
+      <c r="AK47" s="33"/>
+      <c r="AM47" s="34"/>
+      <c r="AO47" s="35"/>
+      <c r="AP47" s="35"/>
+      <c r="AQ47" s="35"/>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M56" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4739,13 +4762,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM40"/>
+  <dimension ref="A1:AN57"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4754,17 +4777,18 @@
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="5" max="6" width="9.140625" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" customWidth="1"/>
     <col min="36" max="36" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -4772,7 +4796,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -4780,52 +4804,52 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="E4" s="39" t="s">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="E4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="25" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="25" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="25" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="27"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="38"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -4920,11 +4944,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -5019,14 +5043,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -5121,8 +5145,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -5228,11 +5252,12 @@
         <v>0</v>
       </c>
       <c r="AK8" s="17"/>
-      <c r="AL8" s="17"/>
-      <c r="AM8" s="17"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="AL8" s="31"/>
+      <c r="AM8" s="31"/>
+      <c r="AN8" s="31"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -5336,11 +5361,12 @@
         <v>0</v>
       </c>
       <c r="AK9" s="17"/>
-      <c r="AL9" s="17"/>
-      <c r="AM9" s="17"/>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="AL9" s="31"/>
+      <c r="AM9" s="31"/>
+      <c r="AN9" s="31"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -5444,11 +5470,12 @@
         <v>0</v>
       </c>
       <c r="AK10" s="17"/>
-      <c r="AL10" s="17"/>
-      <c r="AM10" s="17"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="AL10" s="31"/>
+      <c r="AM10" s="31"/>
+      <c r="AN10" s="31"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -5552,11 +5579,12 @@
         <v>0</v>
       </c>
       <c r="AK11" s="17"/>
-      <c r="AL11" s="17"/>
-      <c r="AM11" s="17"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="AL11" s="31"/>
+      <c r="AM11" s="31"/>
+      <c r="AN11" s="31"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -5639,13 +5667,13 @@
         <v>0</v>
       </c>
       <c r="AC12" s="12">
-        <v>252.8973005344406</v>
+        <v>250.97521489644751</v>
       </c>
       <c r="AD12" s="12">
         <v>0</v>
       </c>
       <c r="AE12" s="12">
-        <v>23.817795898233186</v>
+        <v>27.206038740824212</v>
       </c>
       <c r="AF12" s="11">
         <v>0</v>
@@ -5660,11 +5688,12 @@
         <v>0</v>
       </c>
       <c r="AK12" s="17"/>
-      <c r="AL12" s="17"/>
-      <c r="AM12" s="17"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="AL12" s="31"/>
+      <c r="AM12" s="31"/>
+      <c r="AN12" s="31"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -5747,13 +5776,13 @@
         <v>0</v>
       </c>
       <c r="AC13" s="12">
-        <v>18036.176096752388</v>
+        <v>15791.191311471635</v>
       </c>
       <c r="AD13" s="12">
         <v>0</v>
       </c>
       <c r="AE13" s="12">
-        <v>10949.526655213182</v>
+        <v>6570.8333002596337</v>
       </c>
       <c r="AF13" s="11">
         <v>0</v>
@@ -5768,11 +5797,12 @@
         <v>0</v>
       </c>
       <c r="AK13" s="17"/>
-      <c r="AL13" s="17"/>
-      <c r="AM13" s="17"/>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="AL13" s="31"/>
+      <c r="AM13" s="31"/>
+      <c r="AN13" s="31"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -5855,13 +5885,13 @@
         <v>0</v>
       </c>
       <c r="AC14" s="12">
-        <v>0</v>
+        <v>2.8054317691335942E-2</v>
       </c>
       <c r="AD14" s="12">
         <v>0</v>
       </c>
       <c r="AE14" s="12">
-        <v>0.58128071668327153</v>
+        <v>0.55603854321171253</v>
       </c>
       <c r="AF14" s="11">
         <v>0</v>
@@ -5876,11 +5906,12 @@
         <v>0</v>
       </c>
       <c r="AK14" s="17"/>
-      <c r="AL14" s="17"/>
-      <c r="AM14" s="17"/>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="AL14" s="31"/>
+      <c r="AM14" s="31"/>
+      <c r="AN14" s="31"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -5963,13 +5994,13 @@
         <v>0</v>
       </c>
       <c r="AC15" s="12">
-        <v>1495.1379572521923</v>
+        <v>1680.3408468449684</v>
       </c>
       <c r="AD15" s="12">
         <v>0</v>
       </c>
       <c r="AE15" s="12">
-        <v>325.66057844065494</v>
+        <v>112.67590777366559</v>
       </c>
       <c r="AF15" s="11">
         <v>0</v>
@@ -5985,11 +6016,12 @@
       </c>
       <c r="AJ15" s="17"/>
       <c r="AK15" s="17"/>
-      <c r="AL15" s="17"/>
-      <c r="AM15" s="17"/>
-    </row>
-    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="AL15" s="31"/>
+      <c r="AM15" s="31"/>
+      <c r="AN15" s="31"/>
+    </row>
+    <row r="16" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -6095,11 +6127,12 @@
         <v>0</v>
       </c>
       <c r="AK16" s="17"/>
-      <c r="AL16" s="17"/>
-      <c r="AM16" s="17"/>
-    </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="AL16" s="31"/>
+      <c r="AM16" s="31"/>
+      <c r="AN16" s="31"/>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -6203,11 +6236,12 @@
         <v>0</v>
       </c>
       <c r="AK17" s="17"/>
-      <c r="AL17" s="17"/>
-      <c r="AM17" s="17"/>
-    </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="AL17" s="31"/>
+      <c r="AM17" s="31"/>
+      <c r="AN17" s="31"/>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -6311,11 +6345,12 @@
         <v>0</v>
       </c>
       <c r="AK18" s="17"/>
-      <c r="AL18" s="17"/>
-      <c r="AM18" s="17"/>
-    </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -6419,11 +6454,12 @@
         <v>0</v>
       </c>
       <c r="AK19" s="17"/>
-      <c r="AL19" s="17"/>
-      <c r="AM19" s="17"/>
-    </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="AL19" s="31"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="31"/>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -6527,11 +6563,12 @@
         <v>0</v>
       </c>
       <c r="AK20" s="17"/>
-      <c r="AL20" s="17"/>
-      <c r="AM20" s="17"/>
-    </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31"/>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -6635,11 +6672,12 @@
         <v>0</v>
       </c>
       <c r="AK21" s="17"/>
-      <c r="AL21" s="17"/>
-      <c r="AM21" s="17"/>
-    </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="AL21" s="31"/>
+      <c r="AM21" s="31"/>
+      <c r="AN21" s="31"/>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A22" s="40"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -6743,11 +6781,12 @@
         <v>0</v>
       </c>
       <c r="AK22" s="17"/>
-      <c r="AL22" s="17"/>
-      <c r="AM22" s="17"/>
-    </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="AL22" s="31"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="31"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23" s="42"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -6851,11 +6890,12 @@
         <v>0</v>
       </c>
       <c r="AK23" s="17"/>
-      <c r="AL23" s="17"/>
-      <c r="AM23" s="17"/>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="AL23" s="31"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="31"/>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -6880,16 +6920,16 @@
         <v>818112.77519823459</v>
       </c>
       <c r="I24" s="18">
-        <v>352.4185001695231</v>
+        <v>353.88465737412099</v>
       </c>
       <c r="J24" s="18">
-        <v>39808.454382520133</v>
+        <v>33184.776242285836</v>
       </c>
       <c r="K24" s="18">
-        <v>0.58128071668327153</v>
+        <v>0.58409286090304846</v>
       </c>
       <c r="L24" s="18">
-        <v>6772.8605897242669</v>
+        <v>6745.0788086500543</v>
       </c>
       <c r="M24" s="9">
         <v>-6710.2411205275648</v>
@@ -6940,13 +6980,13 @@
         <v>0</v>
       </c>
       <c r="AC24" s="12">
-        <v>-802703.1198201403</v>
+        <v>-800641.44389313203</v>
       </c>
       <c r="AD24" s="12">
         <v>0</v>
       </c>
       <c r="AE24" s="12">
-        <v>-204412.67687368786</v>
+        <v>-199824.36184873641</v>
       </c>
       <c r="AF24" s="12">
         <v>0</v>
@@ -6961,11 +7001,12 @@
         <v>0</v>
       </c>
       <c r="AK24" s="17"/>
-      <c r="AL24" s="17"/>
-      <c r="AM24" s="17"/>
-    </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="AL24" s="31"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="31"/>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25" s="40"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -7069,11 +7110,12 @@
         <v>0</v>
       </c>
       <c r="AK25" s="17"/>
-      <c r="AL25" s="17"/>
-      <c r="AM25" s="17"/>
-    </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="AL25" s="31"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31"/>
+    </row>
+    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A26" s="40"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -7177,11 +7219,12 @@
         <v>0</v>
       </c>
       <c r="AK26" s="17"/>
-      <c r="AL26" s="17"/>
-      <c r="AM26" s="17"/>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="AL26" s="31"/>
+      <c r="AM26" s="31"/>
+      <c r="AN26" s="31"/>
+    </row>
+    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A27" s="40"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -7285,11 +7328,12 @@
         <v>0</v>
       </c>
       <c r="AK27" s="17"/>
-      <c r="AL27" s="17"/>
-      <c r="AM27" s="17"/>
-    </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="AL27" s="31"/>
+      <c r="AM27" s="31"/>
+      <c r="AN27" s="31"/>
+    </row>
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A28" s="40"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -7393,11 +7437,12 @@
         <v>0</v>
       </c>
       <c r="AK28" s="17"/>
-      <c r="AL28" s="17"/>
-      <c r="AM28" s="17"/>
-    </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="AL28" s="31"/>
+      <c r="AM28" s="31"/>
+      <c r="AN28" s="31"/>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A29" s="40"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -7501,11 +7546,12 @@
         <v>0</v>
       </c>
       <c r="AK29" s="17"/>
-      <c r="AL29" s="17"/>
-      <c r="AM29" s="17"/>
-    </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="AL29" s="31"/>
+      <c r="AM29" s="31"/>
+      <c r="AN29" s="31"/>
+    </row>
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A30" s="40"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -7609,11 +7655,12 @@
         <v>0</v>
       </c>
       <c r="AK30" s="17"/>
-      <c r="AL30" s="17"/>
-      <c r="AM30" s="17"/>
-    </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="AL30" s="31"/>
+      <c r="AM30" s="31"/>
+      <c r="AN30" s="31"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A31" s="42"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -7717,11 +7764,12 @@
         <v>0</v>
       </c>
       <c r="AK31" s="17"/>
-      <c r="AL31" s="17"/>
-      <c r="AM31" s="17"/>
-    </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="AL31" s="31"/>
+      <c r="AM31" s="31"/>
+      <c r="AN31" s="31"/>
+    </row>
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A32" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -7827,11 +7875,12 @@
         <v>0</v>
       </c>
       <c r="AK32" s="17"/>
-      <c r="AL32" s="17"/>
-      <c r="AM32" s="17"/>
-    </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="AL32" s="31"/>
+      <c r="AM32" s="31"/>
+      <c r="AN32" s="31"/>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -7935,11 +7984,12 @@
         <v>0</v>
       </c>
       <c r="AK33" s="17"/>
-      <c r="AL33" s="17"/>
-      <c r="AM33" s="17"/>
-    </row>
-    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="AL33" s="31"/>
+      <c r="AM33" s="31"/>
+      <c r="AN33" s="31"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -8043,11 +8093,12 @@
         <v>0</v>
       </c>
       <c r="AK34" s="17"/>
-      <c r="AL34" s="17"/>
-      <c r="AM34" s="17"/>
-    </row>
-    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="AL34" s="31"/>
+      <c r="AM34" s="31"/>
+      <c r="AN34" s="31"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -8151,11 +8202,12 @@
         <v>0</v>
       </c>
       <c r="AK35" s="17"/>
-      <c r="AL35" s="17"/>
-      <c r="AM35" s="17"/>
-    </row>
-    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="AL35" s="31"/>
+      <c r="AM35" s="31"/>
+      <c r="AN35" s="31"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -8259,11 +8311,12 @@
         <v>0</v>
       </c>
       <c r="AK36" s="17"/>
-      <c r="AL36" s="17"/>
-      <c r="AM36" s="17"/>
-    </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="31"/>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -8367,11 +8420,12 @@
         <v>0</v>
       </c>
       <c r="AK37" s="17"/>
-      <c r="AL37" s="17"/>
-      <c r="AM37" s="17"/>
-    </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A38" s="45"/>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
@@ -8475,10 +8529,281 @@
         <v>0</v>
       </c>
       <c r="AK38" s="17"/>
-      <c r="AL38" s="17"/>
-      <c r="AM38" s="17"/>
-    </row>
-    <row r="40" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+    </row>
+    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="31"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
+    </row>
+    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="29"/>
+      <c r="AF43" s="29"/>
+      <c r="AG43" s="29"/>
+      <c r="AH43" s="29"/>
+      <c r="AI43" s="29"/>
+    </row>
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="29"/>
+      <c r="AC44" s="31"/>
+      <c r="AD44" s="31"/>
+      <c r="AE44" s="31"/>
+      <c r="AF44" s="29"/>
+      <c r="AG44" s="29"/>
+      <c r="AH44" s="29"/>
+      <c r="AI44" s="29"/>
+    </row>
+    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
+      <c r="T45" s="29"/>
+      <c r="AC45" s="29"/>
+      <c r="AD45" s="29"/>
+      <c r="AE45" s="29"/>
+      <c r="AF45" s="29"/>
+      <c r="AG45" s="29"/>
+      <c r="AH45" s="29"/>
+      <c r="AI45" s="29"/>
+    </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
+      <c r="S46" s="29"/>
+      <c r="T46" s="29"/>
+      <c r="AC46" s="29"/>
+      <c r="AD46" s="29"/>
+      <c r="AE46" s="29"/>
+      <c r="AF46" s="29"/>
+      <c r="AG46" s="29"/>
+      <c r="AH46" s="29"/>
+      <c r="AI46" s="29"/>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
+      <c r="AF47" s="29"/>
+      <c r="AG47" s="29"/>
+      <c r="AH47" s="29"/>
+      <c r="AI47" s="29"/>
+    </row>
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
+      <c r="T48" s="29"/>
+      <c r="AC48" s="29"/>
+      <c r="AD48" s="29"/>
+      <c r="AE48" s="29"/>
+      <c r="AF48" s="29"/>
+      <c r="AG48" s="29"/>
+      <c r="AH48" s="29"/>
+      <c r="AI48" s="29"/>
+    </row>
+    <row r="49" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="29"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="29"/>
+      <c r="S49" s="29"/>
+      <c r="T49" s="29"/>
+      <c r="AC49" s="29"/>
+      <c r="AD49" s="29"/>
+      <c r="AE49" s="29"/>
+      <c r="AF49" s="29"/>
+      <c r="AG49" s="29"/>
+      <c r="AH49" s="29"/>
+      <c r="AI49" s="29"/>
+    </row>
+    <row r="50" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
+      <c r="T50" s="29"/>
+      <c r="AC50" s="29"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="29"/>
+      <c r="AF50" s="29"/>
+      <c r="AG50" s="29"/>
+      <c r="AH50" s="29"/>
+      <c r="AI50" s="29"/>
+    </row>
+    <row r="51" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="29"/>
+      <c r="S51" s="29"/>
+      <c r="T51" s="29"/>
+      <c r="AC51" s="29"/>
+      <c r="AD51" s="29"/>
+      <c r="AE51" s="29"/>
+    </row>
+    <row r="52" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M52" s="29"/>
+      <c r="N52" s="29"/>
+      <c r="O52" s="29"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="29"/>
+      <c r="R52" s="29"/>
+      <c r="S52" s="29"/>
+      <c r="T52" s="29"/>
+      <c r="AC52" s="29"/>
+      <c r="AD52" s="29"/>
+      <c r="AE52" s="29"/>
+    </row>
+    <row r="53" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="AC53" s="29"/>
+      <c r="AD53" s="29"/>
+      <c r="AE53" s="29"/>
+    </row>
+    <row r="54" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="N54" s="29"/>
+      <c r="O54" s="29"/>
+      <c r="P54" s="29"/>
+      <c r="Q54" s="29"/>
+      <c r="R54" s="29"/>
+      <c r="S54" s="29"/>
+      <c r="T54" s="29"/>
+      <c r="AC54" s="29"/>
+      <c r="AD54" s="29"/>
+      <c r="AE54" s="29"/>
+      <c r="AF54" s="29"/>
+      <c r="AG54" s="29"/>
+      <c r="AH54" s="29"/>
+      <c r="AI54" s="29"/>
+      <c r="AJ54" s="29"/>
+    </row>
+    <row r="55" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
+      <c r="O55" s="29"/>
+      <c r="P55" s="29"/>
+      <c r="Q55" s="29"/>
+      <c r="R55" s="29"/>
+      <c r="S55" s="29"/>
+      <c r="T55" s="29"/>
+      <c r="AC55" s="29"/>
+      <c r="AD55" s="29"/>
+      <c r="AE55" s="29"/>
+      <c r="AF55" s="29"/>
+      <c r="AG55" s="29"/>
+      <c r="AH55" s="29"/>
+      <c r="AI55" s="29"/>
+      <c r="AJ55" s="29"/>
+    </row>
+    <row r="56" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
+      <c r="O56" s="29"/>
+      <c r="P56" s="29"/>
+      <c r="Q56" s="29"/>
+      <c r="R56" s="29"/>
+      <c r="S56" s="29"/>
+      <c r="T56" s="29"/>
+      <c r="AC56" s="29"/>
+      <c r="AD56" s="29"/>
+      <c r="AE56" s="29"/>
+      <c r="AF56" s="29"/>
+      <c r="AG56" s="29"/>
+      <c r="AH56" s="29"/>
+      <c r="AI56" s="29"/>
+      <c r="AJ56" s="29"/>
+    </row>
+    <row r="57" spans="13:36" x14ac:dyDescent="0.25">
+      <c r="M57" s="29"/>
+      <c r="N57" s="29"/>
+      <c r="O57" s="29"/>
+      <c r="P57" s="29"/>
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29"/>
+      <c r="S57" s="29"/>
+      <c r="T57" s="29"/>
+      <c r="AC57" s="29"/>
+      <c r="AD57" s="29"/>
+      <c r="AE57" s="29"/>
+      <c r="AF57" s="29"/>
+      <c r="AG57" s="29"/>
+      <c r="AH57" s="29"/>
+      <c r="AI57" s="29"/>
+      <c r="AJ57" s="29"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="C6:D6"/>
@@ -8500,13 +8825,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN40"/>
+  <dimension ref="A1:AN41"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8517,12 +8842,12 @@
     <col min="5" max="35" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -8530,7 +8855,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -8538,52 +8863,52 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="E4" s="39" t="s">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="E4" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="25" t="s">
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="26"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
-      <c r="U4" s="25" t="s">
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="26"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="25" t="s">
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="37"/>
+      <c r="AA4" s="37"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="26"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="26"/>
-      <c r="AH4" s="26"/>
-      <c r="AI4" s="27"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C5" s="35" t="s">
+      <c r="AD4" s="37"/>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="37"/>
+      <c r="AG4" s="37"/>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="38"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="47"/>
       <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
@@ -8678,11 +9003,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C6" s="35" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="C6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="1" t="s">
         <v>3</v>
       </c>
@@ -8777,14 +9102,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -8879,8 +9204,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
@@ -8990,7 +9315,7 @@
       </c>
       <c r="AC8" s="10">
         <f>basic_price!AC8+tax_layer!AC8</f>
-        <v>111041.7001363598</v>
+        <v>108705.72593834247</v>
       </c>
       <c r="AD8" s="10">
         <f>basic_price!AD8+tax_layer!AD8</f>
@@ -9002,7 +9327,7 @@
       </c>
       <c r="AF8" s="13">
         <f>basic_price!AF8+tax_layer!AF8</f>
-        <v>1284.4988073369193</v>
+        <v>3620.4730053542426</v>
       </c>
       <c r="AG8" s="13">
         <f>basic_price!AG8+tax_layer!AG8</f>
@@ -9016,9 +9341,12 @@
         <f>basic_price!AI8+tax_layer!AI8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="AL8" s="31"/>
+      <c r="AM8" s="31"/>
+      <c r="AN8" s="31"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="40"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -9126,7 +9454,7 @@
       </c>
       <c r="AC9" s="11">
         <f>basic_price!AC9+tax_layer!AC9</f>
-        <v>2390022.7056223075</v>
+        <v>2257470.6309081297</v>
       </c>
       <c r="AD9" s="11">
         <f>basic_price!AD9+tax_layer!AD9</f>
@@ -9138,7 +9466,7 @@
       </c>
       <c r="AF9" s="12">
         <f>basic_price!AF9+tax_layer!AF9</f>
-        <v>72887.355530256944</v>
+        <v>205439.43024443468</v>
       </c>
       <c r="AG9" s="12">
         <f>basic_price!AG9+tax_layer!AG9</f>
@@ -9152,10 +9480,12 @@
         <f>basic_price!AI9+tax_layer!AI9</f>
         <v>0</v>
       </c>
-      <c r="AL9" s="17"/>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="AL9" s="31"/>
+      <c r="AM9" s="31"/>
+      <c r="AN9" s="31"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
@@ -9263,7 +9593,7 @@
       </c>
       <c r="AC10" s="11">
         <f>basic_price!AC10+tax_layer!AC10</f>
-        <v>53062.363348803236</v>
+        <v>53041.198689549252</v>
       </c>
       <c r="AD10" s="11">
         <f>basic_price!AD10+tax_layer!AD10</f>
@@ -9275,7 +9605,7 @@
       </c>
       <c r="AF10" s="12">
         <f>basic_price!AF10+tax_layer!AF10</f>
-        <v>11.637962265383223</v>
+        <v>32.802621519366994</v>
       </c>
       <c r="AG10" s="12">
         <f>basic_price!AG10+tax_layer!AG10</f>
@@ -9289,10 +9619,12 @@
         <f>basic_price!AI10+tax_layer!AI10</f>
         <v>0</v>
       </c>
-      <c r="AL10" s="17"/>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="AL10" s="31"/>
+      <c r="AM10" s="31"/>
+      <c r="AN10" s="31"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -9400,7 +9732,7 @@
       </c>
       <c r="AC11" s="11">
         <f>basic_price!AC11+tax_layer!AC11</f>
-        <v>5201048.9253524598</v>
+        <v>5143799.6690182388</v>
       </c>
       <c r="AD11" s="11">
         <f>basic_price!AD11+tax_layer!AD11</f>
@@ -9412,7 +9744,7 @@
       </c>
       <c r="AF11" s="12">
         <f>basic_price!AF11+tax_layer!AF11</f>
-        <v>31480.0572474851</v>
+        <v>88729.313581706883</v>
       </c>
       <c r="AG11" s="12">
         <f>basic_price!AG11+tax_layer!AG11</f>
@@ -9426,9 +9758,12 @@
         <f>basic_price!AI11+tax_layer!AI11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="AL11" s="31"/>
+      <c r="AM11" s="31"/>
+      <c r="AN11" s="31"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
@@ -9536,15 +9871,15 @@
       </c>
       <c r="AC12" s="12">
         <f>basic_price!AC12+tax_layer!AC12</f>
-        <v>6436.6521504267066</v>
+        <v>6319.0129988263552</v>
       </c>
       <c r="AD12" s="12">
         <f>basic_price!AD12+tax_layer!AD12</f>
-        <v>113.34784857236332</v>
+        <v>112.4863752732101</v>
       </c>
       <c r="AE12" s="12">
         <f>basic_price!AE12+tax_layer!AE12</f>
-        <v>843.3115521726578</v>
+        <v>963.27833427676069</v>
       </c>
       <c r="AF12" s="11">
         <f>basic_price!AF12+tax_layer!AF12</f>
@@ -9562,9 +9897,12 @@
         <f>basic_price!AI12+tax_layer!AI12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="AL12" s="31"/>
+      <c r="AM12" s="31"/>
+      <c r="AN12" s="31"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -9672,15 +10010,15 @@
       </c>
       <c r="AC13" s="12">
         <f>basic_price!AC13+tax_layer!AC13</f>
-        <v>142304.34263879975</v>
+        <v>172969.08427680435</v>
       </c>
       <c r="AD13" s="12">
         <f>basic_price!AD13+tax_layer!AD13</f>
-        <v>4774.5816843777284</v>
+        <v>4180.283692386055</v>
       </c>
       <c r="AE13" s="12">
         <f>basic_price!AE13+tax_layer!AE13</f>
-        <v>91758.712478374771</v>
+        <v>55064.590692127545</v>
       </c>
       <c r="AF13" s="11">
         <f>basic_price!AF13+tax_layer!AF13</f>
@@ -9698,10 +10036,12 @@
         <f>basic_price!AI13+tax_layer!AI13</f>
         <v>0</v>
       </c>
-      <c r="AL13" s="17"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="AL13" s="31"/>
+      <c r="AM13" s="31"/>
+      <c r="AN13" s="31"/>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -9809,15 +10149,15 @@
       </c>
       <c r="AC14" s="12">
         <f>basic_price!AC14+tax_layer!AC14</f>
-        <v>0</v>
+        <v>0.42911256786485846</v>
       </c>
       <c r="AD14" s="12">
         <f>basic_price!AD14+tax_layer!AD14</f>
-        <v>0</v>
+        <v>3.3192753637309988E-2</v>
       </c>
       <c r="AE14" s="12">
         <f>basic_price!AE14+tax_layer!AE14</f>
-        <v>10.581280716683272</v>
+        <v>10.121787539400881</v>
       </c>
       <c r="AF14" s="11">
         <f>basic_price!AF14+tax_layer!AF14</f>
@@ -9835,9 +10175,12 @@
         <f>basic_price!AI14+tax_layer!AI14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="AL14" s="31"/>
+      <c r="AM14" s="31"/>
+      <c r="AN14" s="31"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
       <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
@@ -9945,15 +10288,15 @@
       </c>
       <c r="AC15" s="12">
         <f>basic_price!AC15+tax_layer!AC15</f>
-        <v>13049.293920868868</v>
+        <v>15189.379044770007</v>
       </c>
       <c r="AD15" s="12">
         <f>basic_price!AD15+tax_layer!AD15</f>
-        <v>6499.2127295343789</v>
+        <v>7304.2708659755572</v>
       </c>
       <c r="AE15" s="12">
         <f>basic_price!AE15+tax_layer!AE15</f>
-        <v>4545.7003342845355</v>
+        <v>1572.7752928680056</v>
       </c>
       <c r="AF15" s="11">
         <f>basic_price!AF15+tax_layer!AF15</f>
@@ -9971,9 +10314,12 @@
         <f>basic_price!AI15+tax_layer!AI15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30" t="s">
+      <c r="AL15" s="31"/>
+      <c r="AM15" s="31"/>
+      <c r="AN15" s="31"/>
+    </row>
+    <row r="16" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="41" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -10109,9 +10455,12 @@
         <f>basic_price!AI16+tax_layer!AI16</f>
         <v>0</v>
       </c>
+      <c r="AL16" s="31"/>
+      <c r="AM16" s="31"/>
+      <c r="AN16" s="31"/>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="3" t="s">
         <v>2</v>
       </c>
@@ -10245,9 +10594,12 @@
         <f>basic_price!AI17+tax_layer!AI17</f>
         <v>0</v>
       </c>
+      <c r="AL17" s="31"/>
+      <c r="AM17" s="31"/>
+      <c r="AN17" s="31"/>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="40"/>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
@@ -10381,9 +10733,12 @@
         <f>basic_price!AI18+tax_layer!AI18</f>
         <v>0</v>
       </c>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
@@ -10517,9 +10872,12 @@
         <f>basic_price!AI19+tax_layer!AI19</f>
         <v>0</v>
       </c>
+      <c r="AL19" s="31"/>
+      <c r="AM19" s="31"/>
+      <c r="AN19" s="31"/>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+      <c r="A20" s="40"/>
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
@@ -10653,9 +11011,12 @@
         <f>basic_price!AI20+tax_layer!AI20</f>
         <v>0</v>
       </c>
+      <c r="AL20" s="31"/>
+      <c r="AM20" s="31"/>
+      <c r="AN20" s="31"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
@@ -10789,9 +11150,12 @@
         <f>basic_price!AI21+tax_layer!AI21</f>
         <v>0</v>
       </c>
+      <c r="AL21" s="31"/>
+      <c r="AM21" s="31"/>
+      <c r="AN21" s="31"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="40"/>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
@@ -10925,11 +11289,12 @@
         <f>basic_price!AI22+tax_layer!AI22</f>
         <v>0</v>
       </c>
-      <c r="AM22" s="17"/>
-      <c r="AN22" s="17"/>
+      <c r="AL22" s="31"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="31"/>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
@@ -11063,11 +11428,12 @@
         <f>basic_price!AI23+tax_layer!AI23</f>
         <v>0</v>
       </c>
-      <c r="AM23" s="17"/>
-      <c r="AN23" s="17"/>
+      <c r="AL23" s="31"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="31"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -11097,19 +11463,19 @@
       </c>
       <c r="I24" s="18">
         <f>basic_price!I24+tax_layer!I24</f>
-        <v>352.4185001695231</v>
+        <v>353.88465737412099</v>
       </c>
       <c r="J24" s="18">
         <f>basic_price!J24+tax_layer!J24</f>
-        <v>39808.454382520133</v>
+        <v>33184.776242285836</v>
       </c>
       <c r="K24" s="18">
         <f>basic_price!K24+tax_layer!K24</f>
-        <v>0.58128071668327153</v>
+        <v>0.58409286090304846</v>
       </c>
       <c r="L24" s="18">
         <f>basic_price!L24+tax_layer!L24</f>
-        <v>6772.8605897242669</v>
+        <v>6745.0788086500543</v>
       </c>
       <c r="M24" s="9">
         <f>basic_price!M24+tax_layer!M24</f>
@@ -11203,9 +11569,12 @@
         <f>basic_price!AI24+tax_layer!AI24</f>
         <v>0</v>
       </c>
+      <c r="AL24" s="31"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="31"/>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
+      <c r="A25" s="40"/>
       <c r="B25" s="3" t="s">
         <v>2</v>
       </c>
@@ -11339,11 +11708,12 @@
         <f>basic_price!AI25+tax_layer!AI25</f>
         <v>0</v>
       </c>
-      <c r="AM25" s="17"/>
-      <c r="AN25" s="17"/>
+      <c r="AL25" s="31"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="31"/>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
+      <c r="A26" s="40"/>
       <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
@@ -11477,9 +11847,12 @@
         <f>basic_price!AI26+tax_layer!AI26</f>
         <v>0</v>
       </c>
+      <c r="AL26" s="31"/>
+      <c r="AM26" s="31"/>
+      <c r="AN26" s="31"/>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
@@ -11613,9 +11986,12 @@
         <f>basic_price!AI27+tax_layer!AI27</f>
         <v>0</v>
       </c>
+      <c r="AL27" s="31"/>
+      <c r="AM27" s="31"/>
+      <c r="AN27" s="31"/>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
+      <c r="A28" s="40"/>
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
@@ -11749,9 +12125,12 @@
         <f>basic_price!AI28+tax_layer!AI28</f>
         <v>0</v>
       </c>
+      <c r="AL28" s="31"/>
+      <c r="AM28" s="31"/>
+      <c r="AN28" s="31"/>
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="40"/>
       <c r="B29" s="3" t="s">
         <v>11</v>
       </c>
@@ -11885,9 +12264,12 @@
         <f>basic_price!AI29+tax_layer!AI29</f>
         <v>0</v>
       </c>
+      <c r="AL29" s="31"/>
+      <c r="AM29" s="31"/>
+      <c r="AN29" s="31"/>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
+      <c r="A30" s="40"/>
       <c r="B30" s="3" t="s">
         <v>11</v>
       </c>
@@ -12021,9 +12403,12 @@
         <f>basic_price!AI30+tax_layer!AI30</f>
         <v>0</v>
       </c>
+      <c r="AL30" s="31"/>
+      <c r="AM30" s="31"/>
+      <c r="AN30" s="31"/>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
@@ -12157,9 +12542,12 @@
         <f>basic_price!AI31+tax_layer!AI31</f>
         <v>0</v>
       </c>
+      <c r="AL31" s="31"/>
+      <c r="AM31" s="31"/>
+      <c r="AN31" s="31"/>
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -12281,7 +12669,7 @@
       </c>
       <c r="AF32" s="12">
         <f>basic_price!AF32+tax_layer!AF32</f>
-        <v>292158.46990567073</v>
+        <v>100000</v>
       </c>
       <c r="AG32" s="12">
         <f>basic_price!AG32+tax_layer!AG32</f>
@@ -12295,9 +12683,12 @@
         <f>basic_price!AI32+tax_layer!AI32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="AL32" s="31"/>
+      <c r="AM32" s="31"/>
+      <c r="AN32" s="31"/>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
       <c r="B33" s="3" t="s">
         <v>2</v>
       </c>
@@ -12373,7 +12764,7 @@
       </c>
       <c r="U33" s="12">
         <f>basic_price!U33+tax_layer!U33</f>
-        <v>1376928.2334026387</v>
+        <v>1370278.2424506797</v>
       </c>
       <c r="V33" s="12">
         <f>basic_price!V33+tax_layer!V33</f>
@@ -12405,7 +12796,7 @@
       </c>
       <c r="AC33" s="12">
         <f>basic_price!AC33+tax_layer!AC33</f>
-        <v>1666879.5468354388</v>
+        <v>1403430.519579133</v>
       </c>
       <c r="AD33" s="12">
         <f>basic_price!AD33+tax_layer!AD33</f>
@@ -12431,9 +12822,12 @@
         <f>basic_price!AI33+tax_layer!AI33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="AL33" s="31"/>
+      <c r="AM33" s="31"/>
+      <c r="AN33" s="31"/>
+    </row>
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A34" s="44"/>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
@@ -12541,11 +12935,11 @@
       </c>
       <c r="AC34" s="12">
         <f>basic_price!AC34+tax_layer!AC34</f>
-        <v>2345817.5384514933</v>
+        <v>2576578.9489849228</v>
       </c>
       <c r="AD34" s="12">
         <f>basic_price!AD34+tax_layer!AD34</f>
-        <v>270308.95007216698</v>
+        <v>0</v>
       </c>
       <c r="AE34" s="12">
         <f>basic_price!AE34+tax_layer!AE34</f>
@@ -12567,9 +12961,12 @@
         <f>basic_price!AI34+tax_layer!AI34</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="AL34" s="31"/>
+      <c r="AM34" s="31"/>
+      <c r="AN34" s="31"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A35" s="44"/>
       <c r="B35" s="3" t="s">
         <v>11</v>
       </c>
@@ -12703,9 +13100,12 @@
         <f>basic_price!AI35+tax_layer!AI35</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+      <c r="AL35" s="31"/>
+      <c r="AM35" s="31"/>
+      <c r="AN35" s="31"/>
+    </row>
+    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
@@ -12825,7 +13225,7 @@
       </c>
       <c r="AF36" s="12">
         <f>basic_price!AF36+tax_layer!AF36</f>
-        <v>1840871.1526996384</v>
+        <v>1840871.1526996386</v>
       </c>
       <c r="AG36" s="12">
         <f>basic_price!AG36+tax_layer!AG36</f>
@@ -12839,9 +13239,12 @@
         <f>basic_price!AI36+tax_layer!AI36</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
+      <c r="AL36" s="31"/>
+      <c r="AM36" s="31"/>
+      <c r="AN36" s="31"/>
+    </row>
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
@@ -12975,9 +13378,12 @@
         <f>basic_price!AI37+tax_layer!AI37</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
+      <c r="AL37" s="31"/>
+      <c r="AM37" s="31"/>
+      <c r="AN37" s="31"/>
+    </row>
+    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A38" s="45"/>
       <c r="B38" s="3" t="s">
         <v>30</v>
       </c>
@@ -13111,8 +13517,11 @@
         <f>basic_price!AI38+tax_layer!AI38</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AL38" s="31"/>
+      <c r="AM38" s="31"/>
+      <c r="AN38" s="31"/>
+    </row>
+    <row r="40" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
@@ -13144,6 +13553,40 @@
       <c r="AG40" s="17"/>
       <c r="AH40" s="17"/>
       <c r="AI40" s="17"/>
+    </row>
+    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="D41" s="29"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="31"/>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31"/>
+      <c r="N41" s="31"/>
+      <c r="O41" s="31"/>
+      <c r="P41" s="31"/>
+      <c r="Q41" s="31"/>
+      <c r="R41" s="31"/>
+      <c r="S41" s="31"/>
+      <c r="T41" s="31"/>
+      <c r="U41" s="31"/>
+      <c r="V41" s="31"/>
+      <c r="W41" s="31"/>
+      <c r="X41" s="31"/>
+      <c r="Y41" s="31"/>
+      <c r="Z41" s="31"/>
+      <c r="AA41" s="31"/>
+      <c r="AB41" s="31"/>
+      <c r="AC41" s="31"/>
+      <c r="AD41" s="31"/>
+      <c r="AE41" s="31"/>
+      <c r="AF41" s="31"/>
+      <c r="AG41" s="31"/>
+      <c r="AH41" s="31"/>
+      <c r="AI41" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>